<commit_message>
Adicion de proximas tareas
</commit_message>
<xml_diff>
--- a/Documentacion/Cronograma Sifweb.xlsx
+++ b/Documentacion/Cronograma Sifweb.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="24780" windowHeight="12150"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="24780" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>Tarea</t>
   </si>
@@ -82,6 +82,30 @@
   </si>
   <si>
     <t>Inserción tabla Proveedor</t>
+  </si>
+  <si>
+    <t>% Cumplimiento</t>
+  </si>
+  <si>
+    <t>abono compra</t>
+  </si>
+  <si>
+    <t>abono venta</t>
+  </si>
+  <si>
+    <t>caja</t>
+  </si>
+  <si>
+    <t>categoria producto</t>
+  </si>
+  <si>
+    <t>valor parametro</t>
+  </si>
+  <si>
+    <t>inventario</t>
+  </si>
+  <si>
+    <t>pago</t>
   </si>
 </sst>
 </file>
@@ -113,7 +137,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -136,83 +160,21 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:J12"/>
+  <dimension ref="B3:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,145 +487,261 @@
     <col min="1" max="1" width="19.5703125" customWidth="1"/>
     <col min="2" max="3" width="11.42578125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="37" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.85546875" customWidth="1"/>
-    <col min="6" max="6" width="36.5703125" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="4:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>2</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>21</v>
       </c>
       <c r="J5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="5">
         <v>41920</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
       </c>
       <c r="J6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="10">
+      <c r="F7" s="5">
         <v>41920</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="H7" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="5">
         <v>41920</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="H8" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="10">
+      <c r="F9" s="5">
         <v>41920</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="5">
         <v>41920</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F11" s="5">
         <v>41920</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="H11" s="3">
+        <v>90</v>
+      </c>
     </row>
     <row r="12" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="5">
         <v>41920</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="H12" s="3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="5">
+        <v>41925</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="5">
+        <v>41925</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="5">
+        <v>41925</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="5">
+        <v>41925</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="5">
+        <v>41925</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="5">
+        <v>41925</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="5">
+        <v>41925</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D3:G3"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G27">
       <formula1>op</formula1>
     </dataValidation>

</xml_diff>